<commit_message>
make BinaryLinear easier to use
</commit_message>
<xml_diff>
--- a/ClassesTaken/edX/2014/LearnFromData/hw05/hw05.xlsx
+++ b/ClassesTaken/edX/2014/LearnFromData/hw05/hw05.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="prob01" sheetId="1" r:id="rId1"/>
+    <sheet name="prob05" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>sigma</t>
   </si>
@@ -36,6 +37,27 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>exp_v</t>
+  </si>
+  <si>
+    <t>exp_u</t>
+  </si>
+  <si>
+    <t>u_exp_v</t>
+  </si>
+  <si>
+    <t>2_v_exp_minus_u</t>
+  </si>
+  <si>
+    <t>E_u_v</t>
   </si>
 </sst>
 </file>
@@ -354,7 +376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -392,4 +414,70 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="B2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C2">
+        <f>EXP($B2)</f>
+        <v>1.0242903178906215</v>
+      </c>
+      <c r="D2">
+        <f>EXP($A2)</f>
+        <v>1.0460278599087169</v>
+      </c>
+      <c r="E2">
+        <f>$A2*$C2</f>
+        <v>4.6093064305077966E-2</v>
+      </c>
+      <c r="F2">
+        <f>2*$B2/$D2</f>
+        <v>4.58878791279888E-2</v>
+      </c>
+      <c r="G2">
+        <f>POWER($E2-$F2, 2)</f>
+        <v>4.2100956897112553E-8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>